<commit_message>
Run updated cleaning script.
</commit_message>
<xml_diff>
--- a/data/duplicates.xlsx
+++ b/data/duplicates.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425246" uniqueCount="2733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554690" uniqueCount="2893">
   <si>
     <t>submissiondate</t>
   </si>
@@ -8217,6 +8217,486 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>secretaire_g</t>
+  </si>
+  <si>
+    <t>date_sg_recruitment</t>
+  </si>
+  <si>
+    <t>secretaire</t>
+  </si>
+  <si>
+    <t>date_secretary_recruitment</t>
+  </si>
+  <si>
+    <t>agent_secretaire</t>
+  </si>
+  <si>
+    <t>temps_plein_secretaire</t>
+  </si>
+  <si>
+    <t>agent_etat_civil</t>
+  </si>
+  <si>
+    <t>date_agent_etat_civil_recruitmen</t>
+  </si>
+  <si>
+    <t>agent_d_etat_civil_recruitment</t>
+  </si>
+  <si>
+    <t>temps_plein_agent_etat_civil</t>
+  </si>
+  <si>
+    <t>comptable</t>
+  </si>
+  <si>
+    <t>date_compatable_recruitment</t>
+  </si>
+  <si>
+    <t>comptable_recruitment</t>
+  </si>
+  <si>
+    <t>temps_plein_comptable</t>
+  </si>
+  <si>
+    <t>regisseur_recettes</t>
+  </si>
+  <si>
+    <t>date_regisseur_recettes_recruitm</t>
+  </si>
+  <si>
+    <t>regisseur_recettes_recruitment</t>
+  </si>
+  <si>
+    <t>temps_plein_regisseur_recettes</t>
+  </si>
+  <si>
+    <t>agent_materiel_transfere</t>
+  </si>
+  <si>
+    <t>date_materiel_transferes_recruit</t>
+  </si>
+  <si>
+    <t>materiel_transferes_recruitment</t>
+  </si>
+  <si>
+    <t>temps_plein_materiel_transfere</t>
+  </si>
+  <si>
+    <t>agent_services_statistiques</t>
+  </si>
+  <si>
+    <t>date_agent_services_statistiques</t>
+  </si>
+  <si>
+    <t>services_statistiques_recruitmen</t>
+  </si>
+  <si>
+    <t>temps_plein_services_statistique</t>
+  </si>
+  <si>
+    <t>agent_service_techniques</t>
+  </si>
+  <si>
+    <t>date_service_techniques_recruitm</t>
+  </si>
+  <si>
+    <t>services_technique_recruitment</t>
+  </si>
+  <si>
+    <t>temps_plein_services_technique</t>
+  </si>
+  <si>
+    <t>agent_affaires_domaniales_foncie</t>
+  </si>
+  <si>
+    <t>date_agent_affaires_domaniales_f</t>
+  </si>
+  <si>
+    <t>temps_plein_affaires_domaniales_</t>
+  </si>
+  <si>
+    <t>suivi_eval_yn</t>
+  </si>
+  <si>
+    <t>suivi_eval_arrete_yn</t>
+  </si>
+  <si>
+    <t>photo_arrete</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_1</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_2</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_3</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_4</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_5</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_6</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_7</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_8</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_9</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_10</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_11</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_12</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_13</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_14</t>
+  </si>
+  <si>
+    <t>image_arrete_suivi_eval_15</t>
+  </si>
+  <si>
+    <t>suivi_eval_work_yn</t>
+  </si>
+  <si>
+    <t>year_suivi_eval_creation</t>
+  </si>
+  <si>
+    <t>who_supported_suivi_eval</t>
+  </si>
+  <si>
+    <t>who_supported_suivi_eval_autre</t>
+  </si>
+  <si>
+    <t>suivi_eval_feedback_yn</t>
+  </si>
+  <si>
+    <t>suivi_eval_feedback_method</t>
+  </si>
+  <si>
+    <t>suivi_eval_feedback_method_autre</t>
+  </si>
+  <si>
+    <t>total_num_scm</t>
+  </si>
+  <si>
+    <t>total_num_ordinary_scm</t>
+  </si>
+  <si>
+    <t>total_num_extraordinary_scm</t>
+  </si>
+  <si>
+    <t>liste_presence_scm_yn</t>
+  </si>
+  <si>
+    <t>session_council_mun</t>
+  </si>
+  <si>
+    <t>total_councilor</t>
+  </si>
+  <si>
+    <t>gender_councilor</t>
+  </si>
+  <si>
+    <t>councilor_attendance_meeting1</t>
+  </si>
+  <si>
+    <t>councilor_attendance_meeting2</t>
+  </si>
+  <si>
+    <t>councilor_attendance_meeting3</t>
+  </si>
+  <si>
+    <t>councilor_attendance_meeting4</t>
+  </si>
+  <si>
+    <t>num_cadre_concertation_meeting20</t>
+  </si>
+  <si>
+    <t>theme_cadre_concertation_meeting</t>
+  </si>
+  <si>
+    <t>financier_cadre_concertation_mee</t>
+  </si>
+  <si>
+    <t>mc_approve_decision_yn</t>
+  </si>
+  <si>
+    <t>num_decision_approved</t>
+  </si>
+  <si>
+    <t>which_decisions_approved</t>
+  </si>
+  <si>
+    <t>local_taxes_2012</t>
+  </si>
+  <si>
+    <t>local_taxes_forecast_2012</t>
+  </si>
+  <si>
+    <t>local_taxes_2013</t>
+  </si>
+  <si>
+    <t>local_taxes_forecast_2013</t>
+  </si>
+  <si>
+    <t>local_taxes_2014</t>
+  </si>
+  <si>
+    <t>local_taxes_2014_amount</t>
+  </si>
+  <si>
+    <t>local_taxes_forecast_2014</t>
+  </si>
+  <si>
+    <t>execution_equipment_procurement_</t>
+  </si>
+  <si>
+    <t>birth_certificates</t>
+  </si>
+  <si>
+    <t>jugements_suppletifs_calculs_201</t>
+  </si>
+  <si>
+    <t>jugements_suppletifs_naissances_</t>
+  </si>
+  <si>
+    <t>supportmats1</t>
+  </si>
+  <si>
+    <t>supportmats2</t>
+  </si>
+  <si>
+    <t>supportmats3</t>
+  </si>
+  <si>
+    <t>satisfactionmats</t>
+  </si>
+  <si>
+    <t>reasonmats</t>
+  </si>
+  <si>
+    <t>supportdrb1</t>
+  </si>
+  <si>
+    <t>supportdrb2</t>
+  </si>
+  <si>
+    <t>supportdrb3</t>
+  </si>
+  <si>
+    <t>satisfactiondrb</t>
+  </si>
+  <si>
+    <t>reasondrb</t>
+  </si>
+  <si>
+    <t>supportdrcmef1</t>
+  </si>
+  <si>
+    <t>supportdrcmef2</t>
+  </si>
+  <si>
+    <t>supportdrcmef3</t>
+  </si>
+  <si>
+    <t>satisfactiondrcmef</t>
+  </si>
+  <si>
+    <t>reasondrcmef</t>
+  </si>
+  <si>
+    <t>supporttr1</t>
+  </si>
+  <si>
+    <t>supporttr2</t>
+  </si>
+  <si>
+    <t>supporttr3</t>
+  </si>
+  <si>
+    <t>satisfactiontr</t>
+  </si>
+  <si>
+    <t>reasontr</t>
+  </si>
+  <si>
+    <t>supportdri1</t>
+  </si>
+  <si>
+    <t>supportdri2</t>
+  </si>
+  <si>
+    <t>supportdri3</t>
+  </si>
+  <si>
+    <t>satisfactiondri</t>
+  </si>
+  <si>
+    <t>reasondri</t>
+  </si>
+  <si>
+    <t>supportdrep1</t>
+  </si>
+  <si>
+    <t>supportdrep2</t>
+  </si>
+  <si>
+    <t>supportdrep3</t>
+  </si>
+  <si>
+    <t>satisfactiondrep</t>
+  </si>
+  <si>
+    <t>reasondrep</t>
+  </si>
+  <si>
+    <t>action_rejetee_yn</t>
+  </si>
+  <si>
+    <t>quel_autorite_tutel</t>
+  </si>
+  <si>
+    <t>action_jugee_yn</t>
+  </si>
+  <si>
+    <t>who_court_favor</t>
+  </si>
+  <si>
+    <t>increase_operational_budget_yn</t>
+  </si>
+  <si>
+    <t>which_new_activity1</t>
+  </si>
+  <si>
+    <t>which_new_activity2</t>
+  </si>
+  <si>
+    <t>which_new_activity3</t>
+  </si>
+  <si>
+    <t>increase_investment_budget</t>
+  </si>
+  <si>
+    <t>which_new_activity21</t>
+  </si>
+  <si>
+    <t>which_new_activity22</t>
+  </si>
+  <si>
+    <t>which_new_activity23</t>
+  </si>
+  <si>
+    <t>trainings_mef</t>
+  </si>
+  <si>
+    <t>trainings_mef_autre</t>
+  </si>
+  <si>
+    <t>taxes_tpp</t>
+  </si>
+  <si>
+    <t>mayor_2006_name</t>
+  </si>
+  <si>
+    <t>mayor_2006_party</t>
+  </si>
+  <si>
+    <t>mayor_2006_phone</t>
+  </si>
+  <si>
+    <t>mayor_2006_replaced_yn</t>
+  </si>
+  <si>
+    <t>mayor2_2006_name</t>
+  </si>
+  <si>
+    <t>mayor2_2006_party</t>
+  </si>
+  <si>
+    <t>mayor2_2006_phone</t>
+  </si>
+  <si>
+    <t>mayor_2012_name</t>
+  </si>
+  <si>
+    <t>mayor_2012_party</t>
+  </si>
+  <si>
+    <t>mayor_2012_phone</t>
+  </si>
+  <si>
+    <t>mayor_2012_replaced_yn</t>
+  </si>
+  <si>
+    <t>mayor2_2012_name</t>
+  </si>
+  <si>
+    <t>mayor2_2012_party</t>
+  </si>
+  <si>
+    <t>mayor2_2012_phone</t>
+  </si>
+  <si>
+    <t>commune1</t>
+  </si>
+  <si>
+    <t>projected_deliveries</t>
+  </si>
+  <si>
+    <t>assisted_deliveries</t>
+  </si>
+  <si>
+    <t>target_vaccination_bcg</t>
+  </si>
+  <si>
+    <t>vaccination_coverage_bcg</t>
+  </si>
+  <si>
+    <t>target_vaccination_vpo3</t>
+  </si>
+  <si>
+    <t>vaccination_coverage_vpo</t>
+  </si>
+  <si>
+    <t>target_vaccination_dtchephib3</t>
+  </si>
+  <si>
+    <t>vaccination_coverage_dtchephib3</t>
+  </si>
+  <si>
+    <t>target_vaccination_var</t>
+  </si>
+  <si>
+    <t>vaccination_coverage_var</t>
+  </si>
+  <si>
+    <t>target_vaccination_vaa</t>
+  </si>
+  <si>
+    <t>vaccination_coverage_vaa</t>
+  </si>
+  <si>
+    <t>information_q</t>
+  </si>
+  <si>
+    <t>note_inf</t>
   </si>
 </sst>
 </file>
@@ -32031,58 +32511,58 @@
         <v>1334</v>
       </c>
       <c r="I1" t="s">
-        <v>1507</v>
+        <v>2878</v>
       </c>
       <c r="J1" t="s">
-        <v>1511</v>
+        <v>109</v>
       </c>
       <c r="K1" t="s">
-        <v>1512</v>
+        <v>110</v>
       </c>
       <c r="L1" t="s">
-        <v>1513</v>
+        <v>111</v>
       </c>
       <c r="M1" t="s">
-        <v>1514</v>
+        <v>2879</v>
       </c>
       <c r="N1" t="s">
-        <v>1515</v>
+        <v>2880</v>
       </c>
       <c r="O1" t="s">
-        <v>1516</v>
+        <v>2881</v>
       </c>
       <c r="P1" t="s">
-        <v>1517</v>
+        <v>2882</v>
       </c>
       <c r="Q1" t="s">
-        <v>1518</v>
+        <v>2883</v>
       </c>
       <c r="R1" t="s">
-        <v>1519</v>
+        <v>2884</v>
       </c>
       <c r="S1" t="s">
-        <v>1520</v>
+        <v>2885</v>
       </c>
       <c r="T1" t="s">
-        <v>1521</v>
+        <v>2886</v>
       </c>
       <c r="U1" t="s">
-        <v>1522</v>
+        <v>2887</v>
       </c>
       <c r="V1" t="s">
-        <v>1523</v>
+        <v>2888</v>
       </c>
       <c r="W1" t="s">
-        <v>1524</v>
+        <v>2889</v>
       </c>
       <c r="X1" t="s">
-        <v>1525</v>
+        <v>2890</v>
       </c>
       <c r="Y1" t="s">
-        <v>174</v>
+        <v>2891</v>
       </c>
       <c r="Z1" t="s">
-        <v>175</v>
+        <v>2892</v>
       </c>
       <c r="AA1" t="s">
         <v>176</v>
@@ -34061,229 +34541,229 @@
         <v>1746</v>
       </c>
       <c r="P1" t="s">
-        <v>1747</v>
+        <v>2733</v>
       </c>
       <c r="Q1" t="s">
-        <v>1748</v>
+        <v>2734</v>
       </c>
       <c r="R1" t="s">
-        <v>1769</v>
+        <v>2735</v>
       </c>
       <c r="S1" t="s">
-        <v>1770</v>
+        <v>2736</v>
       </c>
       <c r="T1" t="s">
-        <v>1790</v>
+        <v>2737</v>
       </c>
       <c r="U1" t="s">
-        <v>1791</v>
+        <v>2738</v>
       </c>
       <c r="V1" t="s">
-        <v>1792</v>
+        <v>2739</v>
       </c>
       <c r="W1" t="s">
-        <v>1793</v>
+        <v>2740</v>
       </c>
       <c r="X1" t="s">
-        <v>1807</v>
+        <v>2741</v>
       </c>
       <c r="Y1" t="s">
-        <v>1808</v>
+        <v>2742</v>
       </c>
       <c r="Z1" t="s">
-        <v>1809</v>
+        <v>2743</v>
       </c>
       <c r="AA1" t="s">
-        <v>1810</v>
+        <v>2744</v>
       </c>
       <c r="AB1" t="s">
-        <v>1824</v>
+        <v>2745</v>
       </c>
       <c r="AC1" t="s">
-        <v>1825</v>
+        <v>2746</v>
       </c>
       <c r="AD1" t="s">
-        <v>1826</v>
+        <v>2747</v>
       </c>
       <c r="AE1" t="s">
-        <v>1827</v>
+        <v>2748</v>
       </c>
       <c r="AF1" t="s">
-        <v>1836</v>
+        <v>2749</v>
       </c>
       <c r="AG1" t="s">
-        <v>1837</v>
+        <v>2750</v>
       </c>
       <c r="AH1" t="s">
-        <v>1838</v>
+        <v>2751</v>
       </c>
       <c r="AI1" t="s">
-        <v>1839</v>
+        <v>2752</v>
       </c>
       <c r="AJ1" t="s">
-        <v>1840</v>
+        <v>2753</v>
       </c>
       <c r="AK1" t="s">
-        <v>1841</v>
+        <v>2754</v>
       </c>
       <c r="AL1" t="s">
-        <v>1842</v>
+        <v>2755</v>
       </c>
       <c r="AM1" t="s">
-        <v>1843</v>
+        <v>2756</v>
       </c>
       <c r="AN1" t="s">
-        <v>1844</v>
+        <v>2757</v>
       </c>
       <c r="AO1" t="s">
-        <v>1845</v>
+        <v>2758</v>
       </c>
       <c r="AP1" t="s">
-        <v>1846</v>
+        <v>2759</v>
       </c>
       <c r="AQ1" t="s">
-        <v>1847</v>
+        <v>2760</v>
       </c>
       <c r="AR1" t="s">
-        <v>1849</v>
+        <v>2761</v>
       </c>
       <c r="AS1" t="s">
-        <v>1850</v>
+        <v>2762</v>
       </c>
       <c r="AT1" t="s">
-        <v>1851</v>
+        <v>2763</v>
       </c>
       <c r="AU1" t="s">
-        <v>1852</v>
+        <v>2764</v>
       </c>
       <c r="AV1" t="s">
         <v>1857</v>
       </c>
       <c r="AW1" t="s">
-        <v>1858</v>
+        <v>2765</v>
       </c>
       <c r="AX1" t="s">
         <v>1859</v>
       </c>
       <c r="AY1" t="s">
-        <v>1860</v>
+        <v>2766</v>
       </c>
       <c r="AZ1" t="s">
-        <v>1861</v>
+        <v>2767</v>
       </c>
       <c r="BA1" t="s">
-        <v>1862</v>
+        <v>2768</v>
       </c>
       <c r="BB1" t="s">
-        <v>1863</v>
+        <v>2769</v>
       </c>
       <c r="BC1" t="s">
-        <v>1881</v>
+        <v>2770</v>
       </c>
       <c r="BD1" t="s">
-        <v>1893</v>
+        <v>2771</v>
       </c>
       <c r="BE1" t="s">
-        <v>1895</v>
+        <v>2772</v>
       </c>
       <c r="BF1" t="s">
-        <v>1897</v>
+        <v>2773</v>
       </c>
       <c r="BG1" t="s">
-        <v>1898</v>
+        <v>2774</v>
       </c>
       <c r="BH1" t="s">
-        <v>1899</v>
+        <v>2775</v>
       </c>
       <c r="BI1" t="s">
-        <v>1900</v>
+        <v>2776</v>
       </c>
       <c r="BJ1" t="s">
-        <v>1901</v>
+        <v>2777</v>
       </c>
       <c r="BK1" t="s">
-        <v>1902</v>
+        <v>2778</v>
       </c>
       <c r="BL1" t="s">
-        <v>1903</v>
+        <v>2779</v>
       </c>
       <c r="BM1" t="s">
-        <v>1904</v>
+        <v>2780</v>
       </c>
       <c r="BN1" t="s">
-        <v>1905</v>
+        <v>2781</v>
       </c>
       <c r="BO1" t="s">
-        <v>1906</v>
+        <v>2782</v>
       </c>
       <c r="BP1" t="s">
-        <v>1907</v>
+        <v>2783</v>
       </c>
       <c r="BQ1" t="s">
-        <v>1908</v>
+        <v>2784</v>
       </c>
       <c r="BR1" t="s">
-        <v>1909</v>
+        <v>2785</v>
       </c>
       <c r="BS1" t="s">
-        <v>1914</v>
+        <v>2786</v>
       </c>
       <c r="BT1" t="s">
-        <v>1915</v>
+        <v>2787</v>
       </c>
       <c r="BU1" t="s">
-        <v>1919</v>
+        <v>2788</v>
       </c>
       <c r="BV1" t="s">
-        <v>1920</v>
+        <v>2789</v>
       </c>
       <c r="BW1" t="s">
-        <v>1927</v>
+        <v>2790</v>
       </c>
       <c r="BX1" t="s">
         <v>1930</v>
       </c>
       <c r="BY1" t="s">
-        <v>1931</v>
+        <v>2791</v>
       </c>
       <c r="BZ1" t="s">
-        <v>1932</v>
+        <v>2792</v>
       </c>
       <c r="CA1" t="s">
-        <v>1933</v>
+        <v>2793</v>
       </c>
       <c r="CB1" t="s">
-        <v>1934</v>
+        <v>2794</v>
       </c>
       <c r="CC1" t="s">
-        <v>1935</v>
+        <v>2795</v>
       </c>
       <c r="CD1" t="s">
-        <v>1936</v>
+        <v>2796</v>
       </c>
       <c r="CE1" t="s">
-        <v>1937</v>
+        <v>2797</v>
       </c>
       <c r="CF1" t="s">
-        <v>1938</v>
+        <v>2798</v>
       </c>
       <c r="CG1" t="s">
-        <v>1939</v>
+        <v>2799</v>
       </c>
       <c r="CH1" t="s">
-        <v>1940</v>
+        <v>2800</v>
       </c>
       <c r="CI1" t="s">
-        <v>1941</v>
+        <v>2801</v>
       </c>
       <c r="CJ1" t="s">
-        <v>1942</v>
+        <v>2802</v>
       </c>
       <c r="CK1" t="s">
-        <v>1943</v>
+        <v>2803</v>
       </c>
       <c r="CL1" t="s">
-        <v>1950</v>
+        <v>2804</v>
       </c>
       <c r="CM1" t="s">
         <v>1951</v>
@@ -34316,235 +34796,235 @@
         <v>1965</v>
       </c>
       <c r="CW1" t="s">
-        <v>1966</v>
+        <v>2805</v>
       </c>
       <c r="CX1" t="s">
-        <v>1967</v>
+        <v>2806</v>
       </c>
       <c r="CY1" t="s">
-        <v>1968</v>
+        <v>2807</v>
       </c>
       <c r="CZ1" t="s">
         <v>1971</v>
       </c>
       <c r="DA1" t="s">
-        <v>1972</v>
+        <v>2808</v>
       </c>
       <c r="DB1" t="s">
-        <v>1973</v>
+        <v>2809</v>
       </c>
       <c r="DC1" t="s">
-        <v>1974</v>
+        <v>2810</v>
       </c>
       <c r="DD1" t="s">
-        <v>1975</v>
+        <v>2811</v>
       </c>
       <c r="DE1" t="s">
-        <v>1976</v>
+        <v>2812</v>
       </c>
       <c r="DF1" t="s">
-        <v>1977</v>
+        <v>2813</v>
       </c>
       <c r="DG1" t="s">
-        <v>1978</v>
+        <v>2814</v>
       </c>
       <c r="DH1" t="s">
-        <v>1979</v>
+        <v>2815</v>
       </c>
       <c r="DI1" t="s">
         <v>1980</v>
       </c>
       <c r="DJ1" t="s">
-        <v>1981</v>
+        <v>2816</v>
       </c>
       <c r="DK1" t="s">
-        <v>1982</v>
+        <v>2817</v>
       </c>
       <c r="DL1" t="s">
-        <v>1983</v>
+        <v>2818</v>
       </c>
       <c r="DM1" t="s">
         <v>1984</v>
       </c>
       <c r="DN1" t="s">
-        <v>1985</v>
+        <v>2819</v>
       </c>
       <c r="DO1" t="s">
-        <v>2019</v>
+        <v>2820</v>
       </c>
       <c r="DP1" t="s">
-        <v>2040</v>
+        <v>2821</v>
       </c>
       <c r="DQ1" t="s">
-        <v>2053</v>
+        <v>2822</v>
       </c>
       <c r="DR1" t="s">
-        <v>2054</v>
+        <v>2823</v>
       </c>
       <c r="DS1" t="s">
-        <v>2066</v>
+        <v>2824</v>
       </c>
       <c r="DT1" t="s">
-        <v>2097</v>
+        <v>2825</v>
       </c>
       <c r="DU1" t="s">
-        <v>2117</v>
+        <v>2826</v>
       </c>
       <c r="DV1" t="s">
-        <v>2125</v>
+        <v>2827</v>
       </c>
       <c r="DW1" t="s">
-        <v>2126</v>
+        <v>2828</v>
       </c>
       <c r="DX1" t="s">
-        <v>2131</v>
+        <v>2829</v>
       </c>
       <c r="DY1" t="s">
-        <v>2164</v>
+        <v>2830</v>
       </c>
       <c r="DZ1" t="s">
-        <v>2191</v>
+        <v>2831</v>
       </c>
       <c r="EA1" t="s">
-        <v>2207</v>
+        <v>2832</v>
       </c>
       <c r="EB1" t="s">
-        <v>2208</v>
+        <v>2833</v>
       </c>
       <c r="EC1" t="s">
-        <v>2226</v>
+        <v>2834</v>
       </c>
       <c r="ED1" t="s">
-        <v>2251</v>
+        <v>2835</v>
       </c>
       <c r="EE1" t="s">
-        <v>2274</v>
+        <v>2836</v>
       </c>
       <c r="EF1" t="s">
-        <v>2288</v>
+        <v>2837</v>
       </c>
       <c r="EG1" t="s">
-        <v>2289</v>
+        <v>2838</v>
       </c>
       <c r="EH1" t="s">
-        <v>2296</v>
+        <v>2839</v>
       </c>
       <c r="EI1" t="s">
-        <v>2317</v>
+        <v>2840</v>
       </c>
       <c r="EJ1" t="s">
-        <v>2332</v>
+        <v>2841</v>
       </c>
       <c r="EK1" t="s">
-        <v>2346</v>
+        <v>2842</v>
       </c>
       <c r="EL1" t="s">
-        <v>2347</v>
+        <v>2843</v>
       </c>
       <c r="EM1" t="s">
-        <v>2356</v>
+        <v>2844</v>
       </c>
       <c r="EN1" t="s">
-        <v>2381</v>
+        <v>2845</v>
       </c>
       <c r="EO1" t="s">
-        <v>2396</v>
+        <v>2846</v>
       </c>
       <c r="EP1" t="s">
-        <v>2403</v>
+        <v>2847</v>
       </c>
       <c r="EQ1" t="s">
-        <v>2404</v>
+        <v>2848</v>
       </c>
       <c r="ER1" t="s">
-        <v>2415</v>
+        <v>2849</v>
       </c>
       <c r="ES1" t="s">
-        <v>2416</v>
+        <v>2850</v>
       </c>
       <c r="ET1" t="s">
-        <v>2421</v>
+        <v>2851</v>
       </c>
       <c r="EU1" t="s">
-        <v>2422</v>
+        <v>2852</v>
       </c>
       <c r="EV1" t="s">
-        <v>2423</v>
+        <v>2853</v>
       </c>
       <c r="EW1" t="s">
-        <v>2424</v>
+        <v>2854</v>
       </c>
       <c r="EX1" t="s">
-        <v>2440</v>
+        <v>2855</v>
       </c>
       <c r="EY1" t="s">
-        <v>2451</v>
+        <v>2856</v>
       </c>
       <c r="EZ1" t="s">
-        <v>2457</v>
+        <v>2857</v>
       </c>
       <c r="FA1" t="s">
-        <v>2458</v>
+        <v>2858</v>
       </c>
       <c r="FB1" t="s">
-        <v>2470</v>
+        <v>2859</v>
       </c>
       <c r="FC1" t="s">
-        <v>2480</v>
+        <v>2860</v>
       </c>
       <c r="FD1" t="s">
-        <v>2487</v>
+        <v>2861</v>
       </c>
       <c r="FE1" t="s">
-        <v>2491</v>
+        <v>2862</v>
       </c>
       <c r="FF1" t="s">
-        <v>2504</v>
+        <v>2863</v>
       </c>
       <c r="FG1" t="s">
         <v>2505</v>
       </c>
       <c r="FH1" t="s">
-        <v>2506</v>
+        <v>2864</v>
       </c>
       <c r="FI1" t="s">
-        <v>2549</v>
+        <v>2865</v>
       </c>
       <c r="FJ1" t="s">
-        <v>2561</v>
+        <v>2866</v>
       </c>
       <c r="FK1" t="s">
-        <v>2562</v>
+        <v>2867</v>
       </c>
       <c r="FL1" t="s">
-        <v>2563</v>
+        <v>2868</v>
       </c>
       <c r="FM1" t="s">
-        <v>2569</v>
+        <v>2869</v>
       </c>
       <c r="FN1" t="s">
-        <v>2571</v>
+        <v>2870</v>
       </c>
       <c r="FO1" t="s">
-        <v>2572</v>
+        <v>2871</v>
       </c>
       <c r="FP1" t="s">
-        <v>2596</v>
+        <v>2872</v>
       </c>
       <c r="FQ1" t="s">
-        <v>2604</v>
+        <v>2873</v>
       </c>
       <c r="FR1" t="s">
-        <v>2605</v>
+        <v>2874</v>
       </c>
       <c r="FS1" t="s">
-        <v>2606</v>
+        <v>2875</v>
       </c>
       <c r="FT1" t="s">
-        <v>2620</v>
+        <v>2876</v>
       </c>
       <c r="FU1" t="s">
-        <v>2625</v>
+        <v>2877</v>
       </c>
       <c r="FV1" t="s">
         <v>176</v>

</xml_diff>